<commit_message>
feat: Funcionalitat de l'opció 1
</commit_message>
<xml_diff>
--- a/tests/Pla de proves.xlsx
+++ b/tests/Pla de proves.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jairo\Documents\Programació\Java\PE\PE03\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A007CFFB-7125-4DB9-BD15-194E305AC9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC997A01-62B3-445B-B03A-D80E7F838114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -270,7 +270,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -316,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -324,11 +324,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -337,10 +336,22 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -364,6 +375,9 @@
       </font>
     </dxf>
     <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -382,22 +396,7 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -465,13 +464,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1521B260-B202-48BE-AA01-CE1DC9CF3870}" name="Taula14" displayName="Taula14" ref="A1:G8" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1521B260-B202-48BE-AA01-CE1DC9CF3870}" name="Taula14" displayName="Taula14" ref="A1:G8" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:G8" xr:uid="{95658AF5-3DCB-4334-BBB7-DBA085D3D919}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4D315BBF-6E6E-437E-B134-144F06AFFC10}" name="id"/>
     <tableColumn id="2" xr3:uid="{9143D183-7D3B-4F84-B063-9BDE68EA1A76}" name="Prova (descripció)"/>
     <tableColumn id="7" xr3:uid="{FF6BCAB4-CE8F-43E2-BC04-A3FEC6422617}" name="Valors admessos"/>
-    <tableColumn id="3" xr3:uid="{8CDC49C1-EC78-400B-8F6E-943969B08D76}" name="Valor d'entrada" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8CDC49C1-EC78-400B-8F6E-943969B08D76}" name="Valor d'entrada" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{B0B088F2-A476-4E30-A46F-C0E87910AFA6}" name="Valor de sortida"/>
     <tableColumn id="5" xr3:uid="{0D9F2321-DB01-4306-A6C2-A9458D668585}" name="Resultat esperat"/>
     <tableColumn id="6" xr3:uid="{127DAC14-64D7-481E-9A0C-77F9D5B8C00D}" name="Estat de la prova"/>
@@ -487,7 +486,7 @@
     <tableColumn id="1" xr3:uid="{37E2D2BB-DE71-4BA5-AAE7-A432D3E23649}" name="id"/>
     <tableColumn id="2" xr3:uid="{06DA353C-EB0E-44AF-89F2-200D7002312D}" name="Prova (descripció)"/>
     <tableColumn id="7" xr3:uid="{D800E1CC-FE7D-4EFD-9FE7-435AF31E5F1B}" name="Valors admessos"/>
-    <tableColumn id="3" xr3:uid="{0D1F0031-3AE1-4926-9CA4-21E7980541B7}" name="Valor d'entrada" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{0D1F0031-3AE1-4926-9CA4-21E7980541B7}" name="Valor d'entrada" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{80BE2B9E-E668-40CE-B981-B569E19C1D77}" name="Valor de sortida"/>
     <tableColumn id="5" xr3:uid="{BDA66426-6B8D-46B3-B07E-D5836FD46138}" name="Resultat esperat"/>
     <tableColumn id="6" xr3:uid="{61FAB909-8A6E-491F-A84A-9D348AD9ECBB}" name="Estat de la prova"/>
@@ -497,13 +496,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8C96A2DA-29EB-49B7-A02A-44C04CCEFFAB}" name="Taula16" displayName="Taula16" ref="A1:G11" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8C96A2DA-29EB-49B7-A02A-44C04CCEFFAB}" name="Taula16" displayName="Taula16" ref="A1:G11" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:G11" xr:uid="{95658AF5-3DCB-4334-BBB7-DBA085D3D919}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{947B1E39-913D-4DAE-937A-55A9E0C46D5A}" name="id"/>
     <tableColumn id="2" xr3:uid="{7CAE60B0-3DC8-4CCF-BC32-54A2D99DB297}" name="Prova (descripció)"/>
     <tableColumn id="7" xr3:uid="{EA187BB9-3B0A-42E5-A343-9E7D301B8944}" name="Valors admessos"/>
-    <tableColumn id="3" xr3:uid="{1025DBAE-8F16-4367-999E-E5E7782F5D16}" name="Valor d'entrada" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{1025DBAE-8F16-4367-999E-E5E7782F5D16}" name="Valor d'entrada" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{5FEA9720-91BB-4C2D-ABB3-BB784B7CD96F}" name="Valor de sortida"/>
     <tableColumn id="5" xr3:uid="{FB3CB670-FFD4-492C-BD7D-2040B5018ADB}" name="Resultat esperat"/>
     <tableColumn id="6" xr3:uid="{45418F3B-FB24-49DC-9CA4-6266E95AB04E}" name="Estat de la prova"/>
@@ -513,7 +512,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95658AF5-3DCB-4334-BBB7-DBA085D3D919}" name="Taula1" displayName="Taula1" ref="A1:G2" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95658AF5-3DCB-4334-BBB7-DBA085D3D919}" name="Taula1" displayName="Taula1" ref="A1:G2" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:G2" xr:uid="{95658AF5-3DCB-4334-BBB7-DBA085D3D919}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D8413AED-16B9-4E02-B212-241A98EB60C2}" name="id"/>
@@ -1202,7 +1201,6 @@
       <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
@@ -1221,7 +1219,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1424,7 +1422,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="2"/>
@@ -1446,7 +1444,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>50000000000</v>
       </c>
       <c r="E11" t="s">
@@ -1677,11 +1675,11 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>69</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>1</v>
       </c>
       <c r="F10" t="s">
@@ -1699,7 +1697,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>50000000000</v>
       </c>
       <c r="E11" t="s">

</xml_diff>